<commit_message>
finished clean, need data engineering
</commit_message>
<xml_diff>
--- a/Weather_stations/Weather_stations/Yeovilton.xlsx
+++ b/Weather_stations/Weather_stations/Yeovilton.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paxton615/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paxton615/Github_Personal/Notes/Notes/Weather_stations/Weather_stations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D061E83B-022C-4B42-9CE5-5D7D1EEC1E01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C759AA-80DC-A144-A763-0C102CD3C3FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1000" windowWidth="27840" windowHeight="16180" xr2:uid="{71FE5619-BED9-D841-9521-13EEDCA7E349}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="239">
   <si>
     <t>yyyy</t>
   </si>
@@ -694,9 +694,6 @@
   </si>
   <si>
     <t>43.2*</t>
-  </si>
-  <si>
-    <t>Provisional</t>
   </si>
   <si>
     <t>65.6#</t>
@@ -1124,7 +1121,7 @@
   <dimension ref="A1:J693"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1154,7 +1151,15 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J1" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1"/>
@@ -1174,13 +1179,13 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" t="s">
         <v>236</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>237</v>
-      </c>
-      <c r="J2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1206,7 +1211,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I3">
         <v>51.006</v>
@@ -17437,9 +17442,7 @@
       <c r="G679" t="s">
         <v>222</v>
       </c>
-      <c r="H679" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="H679" s="1"/>
     </row>
     <row r="680" spans="1:8">
       <c r="A680" s="1">
@@ -17461,11 +17464,9 @@
         <v>61.8</v>
       </c>
       <c r="G680" t="s">
-        <v>224</v>
-      </c>
-      <c r="H680" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="H680" s="1"/>
     </row>
     <row r="681" spans="1:8">
       <c r="A681" s="1">
@@ -17487,11 +17488,9 @@
         <v>27.8</v>
       </c>
       <c r="G681" t="s">
-        <v>225</v>
-      </c>
-      <c r="H681" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="H681" s="1"/>
     </row>
     <row r="682" spans="1:8">
       <c r="A682" s="1">
@@ -17513,11 +17512,9 @@
         <v>17.2</v>
       </c>
       <c r="G682" t="s">
-        <v>226</v>
-      </c>
-      <c r="H682" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="H682" s="1"/>
     </row>
     <row r="683" spans="1:8">
       <c r="A683" s="1">
@@ -17539,11 +17536,9 @@
         <v>98.2</v>
       </c>
       <c r="G683" t="s">
-        <v>227</v>
-      </c>
-      <c r="H683" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="H683" s="1"/>
     </row>
     <row r="684" spans="1:8">
       <c r="A684" s="1">
@@ -17565,11 +17560,9 @@
         <v>42</v>
       </c>
       <c r="G684" t="s">
-        <v>228</v>
-      </c>
-      <c r="H684" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="H684" s="1"/>
     </row>
     <row r="685" spans="1:8">
       <c r="A685" s="1">
@@ -17591,11 +17584,9 @@
         <v>76</v>
       </c>
       <c r="G685" t="s">
-        <v>229</v>
-      </c>
-      <c r="H685" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="H685" s="1"/>
     </row>
     <row r="686" spans="1:8">
       <c r="A686" s="1">
@@ -17617,11 +17608,9 @@
         <v>30.2</v>
       </c>
       <c r="G686" t="s">
-        <v>230</v>
-      </c>
-      <c r="H686" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="H686" s="1"/>
     </row>
     <row r="687" spans="1:8">
       <c r="A687" s="1">
@@ -17643,11 +17632,9 @@
         <v>44</v>
       </c>
       <c r="G687" t="s">
-        <v>231</v>
-      </c>
-      <c r="H687" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="H687" s="1"/>
     </row>
     <row r="688" spans="1:8">
       <c r="A688" s="1">
@@ -17669,11 +17656,9 @@
         <v>115.8</v>
       </c>
       <c r="G688" t="s">
-        <v>232</v>
-      </c>
-      <c r="H688" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="H688" s="1"/>
     </row>
     <row r="689" spans="1:8">
       <c r="A689" s="1">
@@ -17695,11 +17680,9 @@
         <v>12.2</v>
       </c>
       <c r="G689" t="s">
-        <v>233</v>
-      </c>
-      <c r="H689" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="H689" s="1"/>
     </row>
     <row r="690" spans="1:8">
       <c r="A690" s="1">
@@ -17723,9 +17706,7 @@
       <c r="G690" t="s">
         <v>103</v>
       </c>
-      <c r="H690" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="H690" s="1"/>
     </row>
     <row r="691" spans="1:8">
       <c r="A691" s="1">
@@ -17747,11 +17728,9 @@
         <v>22.4</v>
       </c>
       <c r="G691" t="s">
-        <v>234</v>
-      </c>
-      <c r="H691" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="H691" s="1"/>
     </row>
     <row r="692" spans="1:8">
       <c r="A692" s="1">
@@ -17775,9 +17754,7 @@
       <c r="G692" t="s">
         <v>146</v>
       </c>
-      <c r="H692" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="H692" s="1"/>
     </row>
     <row r="693" spans="1:8">
       <c r="A693" s="1">
@@ -17799,11 +17776,9 @@
         <v>49.2</v>
       </c>
       <c r="G693" t="s">
-        <v>235</v>
-      </c>
-      <c r="H693" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="H693" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>